<commit_message>
update validators and test cases
</commit_message>
<xml_diff>
--- a/test_data/Excel_QUALIFICATIONS.xlsx
+++ b/test_data/Excel_QUALIFICATIONS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AEGIS-backend-NodeJS\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD93858C-F252-4932-9844-F72E1722F44C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA5031C8-7A0D-4B88-9EFB-2A1F1DF600EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1802" uniqueCount="905">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1808" uniqueCount="905">
   <si>
     <t>Callsign</t>
   </si>
@@ -3110,10 +3110,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B901"/>
+  <dimension ref="A1:B904"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A880" workbookViewId="0">
-      <selection activeCell="D896" sqref="D896"/>
+    <sheetView tabSelected="1" topLeftCell="A888" workbookViewId="0">
+      <selection activeCell="J904" sqref="J904"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10326,6 +10326,30 @@
         <v>904</v>
       </c>
     </row>
+    <row r="902" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A902" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B902" s="1" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="903" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A903" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B903" s="1" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="904" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A904" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B904" s="1" t="s">
+        <v>902</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>